<commit_message>
Create one Data Model File. Added my data to one sheet.
</commit_message>
<xml_diff>
--- a/Capstone Project/Monika/Repair Costs.xlsx
+++ b/Capstone Project/Monika/Repair Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mszuc\Desktop\Capstone-Project-Data-Modeling-and-PowerBI\Capstone Project\Monika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565E2DA4-96C2-4B2F-BF2D-12F5D9968783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9722C6-8BED-4431-8E27-5C033100DF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{ED117939-1D2E-4498-B130-96B64592D033}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED117939-1D2E-4498-B130-96B64592D033}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,11 +763,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6105DF2C-7430-48BF-A45E-C623D48AA4A1}">
   <dimension ref="A2:CL63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="30.86328125" customWidth="1"/>
     <col min="2" max="3" width="21.6640625" customWidth="1"/>
@@ -804,14 +804,14 @@
     <col min="37" max="37" width="18.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" ht="38.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:25" ht="38.25">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:25" ht="18.600000000000001" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -829,7 +829,7 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
     </row>
-    <row r="4" spans="1:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:25" ht="18.600000000000001" customHeight="1">
       <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25" ht="18.600000000000001" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -896,7 +896,7 @@
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:25" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:25" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A6" s="10">
         <v>600</v>
       </c>
@@ -947,7 +947,7 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25" ht="18.600000000000001" customHeight="1">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -972,7 +972,7 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
     </row>
-    <row r="8" spans="1:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" ht="18.600000000000001" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>33</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:25" ht="18.600000000000001" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -1030,7 +1030,7 @@
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
     </row>
-    <row r="10" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" ht="18" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>35</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -1077,7 +1077,7 @@
       <c r="T12" s="24"/>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25">
       <c r="A13" s="23" t="s">
         <v>28</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25">
       <c r="A14" s="14">
         <v>2019</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>8794110</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25">
       <c r="A15" s="14"/>
       <c r="B15" s="7">
         <v>38970</v>
@@ -1250,7 +1250,7 @@
         <v>9937350</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25">
       <c r="A16" s="14"/>
       <c r="B16" s="7">
         <v>35825</v>
@@ -1303,7 +1303,7 @@
         <v>20420250</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21">
       <c r="A17" s="14"/>
       <c r="B17" s="7">
         <v>24213</v>
@@ -1368,7 +1368,7 @@
         <v>19346187</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21">
       <c r="A18" s="14"/>
       <c r="B18" s="7">
         <v>26345</v>
@@ -1427,7 +1427,7 @@
         <v>39122325</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21">
       <c r="A19" s="14"/>
       <c r="B19" s="7">
         <v>25968</v>
@@ -1480,7 +1480,7 @@
         <v>12334800</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21">
       <c r="A20" s="14"/>
       <c r="B20" s="7">
         <v>28322</v>
@@ -1539,7 +1539,7 @@
         <v>8921430</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21">
       <c r="A21" s="15" t="s">
         <v>29</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>118876452</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21">
       <c r="A22" s="14">
         <v>2018</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>13946310</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21">
       <c r="A23" s="14"/>
       <c r="B23" s="7">
         <v>38253</v>
@@ -1729,7 +1729,7 @@
         <v>53133417</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21">
       <c r="A24" s="14"/>
       <c r="B24" s="7">
         <v>35347</v>
@@ -1788,7 +1788,7 @@
         <v>63978070</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21">
       <c r="A25" s="14"/>
       <c r="B25" s="7">
         <v>23254</v>
@@ -1847,7 +1847,7 @@
         <v>29979181</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21">
       <c r="A26" s="14"/>
       <c r="B26" s="7">
         <v>25421</v>
@@ -1903,7 +1903,7 @@
         <v>20209695</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21">
       <c r="A27" s="14"/>
       <c r="B27" s="7">
         <v>25180</v>
@@ -1953,7 +1953,7 @@
         <v>19640400</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21">
       <c r="A28" s="14"/>
       <c r="B28" s="7">
         <v>27256</v>
@@ -2012,7 +2012,7 @@
         <v>57782720</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21">
       <c r="A29" s="15" t="s">
         <v>31</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>258669793</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21">
       <c r="A30" s="14">
         <v>2017</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>27218520</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21">
       <c r="A31" s="14"/>
       <c r="B31" s="7">
         <v>37463</v>
@@ -2208,7 +2208,7 @@
         <v>85602955</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21">
       <c r="A32" s="14"/>
       <c r="B32" s="7">
         <v>34774</v>
@@ -2267,7 +2267,7 @@
         <v>42076540</v>
       </c>
     </row>
-    <row r="33" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:90">
       <c r="A33" s="14"/>
       <c r="B33" s="7">
         <v>22597</v>
@@ -2332,7 +2332,7 @@
         <v>53984233</v>
       </c>
     </row>
-    <row r="34" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:90">
       <c r="A34" s="14"/>
       <c r="B34" s="7">
         <v>24520</v>
@@ -2388,7 +2388,7 @@
         <v>27339800</v>
       </c>
     </row>
-    <row r="35" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:90">
       <c r="A35" s="14"/>
       <c r="B35" s="7">
         <v>23581</v>
@@ -2447,7 +2447,7 @@
         <v>44948150</v>
       </c>
     </row>
-    <row r="36" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:90">
       <c r="A36" s="14"/>
       <c r="B36" s="7">
         <v>26077</v>
@@ -2503,7 +2503,7 @@
         <v>29571318</v>
       </c>
     </row>
-    <row r="37" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:90">
       <c r="A37" s="15" t="s">
         <v>30</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>310741516</v>
       </c>
     </row>
-    <row r="38" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:90">
       <c r="A38" s="14">
         <v>2016</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>26680500</v>
       </c>
     </row>
-    <row r="39" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:90">
       <c r="A39" s="14"/>
       <c r="B39" s="7">
         <v>36189</v>
@@ -2755,7 +2755,7 @@
       <c r="CK39" s="17"/>
       <c r="CL39" s="17"/>
     </row>
-    <row r="40" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:90">
       <c r="A40" s="14"/>
       <c r="B40" s="1">
         <v>33508</v>
@@ -2882,7 +2882,7 @@
       <c r="CK40" s="17"/>
       <c r="CL40" s="17"/>
     </row>
-    <row r="41" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:90">
       <c r="A41" s="14"/>
       <c r="B41" s="1">
         <v>21644</v>
@@ -3006,7 +3006,7 @@
       <c r="CK41" s="17"/>
       <c r="CL41" s="17"/>
     </row>
-    <row r="42" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:90">
       <c r="A42" s="14"/>
       <c r="B42" s="1">
         <v>22911</v>
@@ -3127,7 +3127,7 @@
       <c r="CK42" s="17"/>
       <c r="CL42" s="17"/>
     </row>
-    <row r="43" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:90">
       <c r="A43" s="14"/>
       <c r="B43" s="1">
         <v>24191</v>
@@ -3248,7 +3248,7 @@
       <c r="CK43" s="17"/>
       <c r="CL43" s="17"/>
     </row>
-    <row r="44" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:90">
       <c r="A44" s="14"/>
       <c r="B44" s="1">
         <v>25412</v>
@@ -3370,7 +3370,7 @@
       <c r="CK44" s="17"/>
       <c r="CL44" s="17"/>
     </row>
-    <row r="45" spans="1:90" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:90" s="2" customFormat="1">
       <c r="A45" s="15" t="s">
         <v>40</v>
       </c>
@@ -3517,7 +3517,7 @@
       <c r="CK45" s="17"/>
       <c r="CL45" s="17"/>
     </row>
-    <row r="46" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:90">
       <c r="A46" s="14">
         <v>2015</v>
       </c>
@@ -3638,7 +3638,7 @@
       <c r="CK46" s="17"/>
       <c r="CL46" s="17"/>
     </row>
-    <row r="47" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:90">
       <c r="A47" s="1"/>
       <c r="B47" s="1">
         <v>34008</v>
@@ -3766,7 +3766,7 @@
       <c r="CK47" s="17"/>
       <c r="CL47" s="17"/>
     </row>
-    <row r="48" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:90">
       <c r="A48" s="1"/>
       <c r="B48" s="1">
         <v>31395</v>
@@ -3894,7 +3894,7 @@
       <c r="CK48" s="17"/>
       <c r="CL48" s="17"/>
     </row>
-    <row r="49" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:90">
       <c r="A49" s="1"/>
       <c r="B49" s="1">
         <v>21069</v>
@@ -4025,7 +4025,7 @@
       <c r="CK49" s="17"/>
       <c r="CL49" s="17"/>
     </row>
-    <row r="50" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:90">
       <c r="A50" s="14"/>
       <c r="B50" s="1">
         <v>23049</v>
@@ -4147,7 +4147,7 @@
       <c r="CK50" s="17"/>
       <c r="CL50" s="17"/>
     </row>
-    <row r="51" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:90">
       <c r="A51" s="14"/>
       <c r="B51" s="1">
         <v>22879</v>
@@ -4281,7 +4281,7 @@
       <c r="CK51" s="17"/>
       <c r="CL51" s="17"/>
     </row>
-    <row r="52" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:90">
       <c r="A52" s="14"/>
       <c r="B52" s="1">
         <v>23515</v>
@@ -4403,7 +4403,7 @@
       <c r="CK52" s="17"/>
       <c r="CL52" s="17"/>
     </row>
-    <row r="53" spans="1:90" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:90" s="2" customFormat="1">
       <c r="A53" s="15" t="s">
         <v>39</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>13025760</v>
       </c>
       <c r="P53" s="21">
-        <f t="shared" ref="P53:S53" si="25">SUM(P46:P52)</f>
+        <f t="shared" ref="P53:R53" si="25">SUM(P46:P52)</f>
         <v>19827720</v>
       </c>
       <c r="Q53" s="21">
@@ -4550,7 +4550,7 @@
       <c r="CK53" s="17"/>
       <c r="CL53" s="17"/>
     </row>
-    <row r="54" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:90">
       <c r="A54" s="16" t="s">
         <v>10</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>74200320</v>
       </c>
       <c r="P54" s="22">
-        <f t="shared" ref="P54:S54" si="26">SUM(P21+P29+P37+P45+P53)</f>
+        <f t="shared" ref="P54:R54" si="26">SUM(P21+P29+P37+P45+P53)</f>
         <v>151408800</v>
       </c>
       <c r="Q54" s="22">
@@ -4698,7 +4698,7 @@
       <c r="CK54" s="17"/>
       <c r="CL54" s="17"/>
     </row>
-    <row r="55" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:90">
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
       <c r="X55" s="17"/>
@@ -4769,29 +4769,29 @@
       <c r="CK55" s="17"/>
       <c r="CL55" s="17"/>
     </row>
-    <row r="56" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:90">
       <c r="V56" s="17"/>
       <c r="W56" s="17"/>
       <c r="X56" s="17"/>
       <c r="Y56" s="17"/>
       <c r="Z56" s="17"/>
     </row>
-    <row r="57" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:90">
       <c r="B57" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:90">
       <c r="B58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:90">
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
     </row>
-    <row r="63" spans="1:90" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:90">
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>

</xml_diff>